<commit_message>
Update README, add performance test scaled image.
</commit_message>
<xml_diff>
--- a/Part1/resources/Performance Comparison.xlsx
+++ b/Part1/resources/Performance Comparison.xlsx
@@ -168,9 +168,6 @@
             <a:solidFill>
               <a:schemeClr val="accent3"/>
             </a:solidFill>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -276,9 +273,6 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -363,11 +357,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45043200"/>
-        <c:axId val="110169472"/>
+        <c:axId val="115286528"/>
+        <c:axId val="69768832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45043200"/>
+        <c:axId val="115286528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +400,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110169472"/>
+        <c:crossAx val="69768832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -414,7 +408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110169472"/>
+        <c:axId val="69768832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +459,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45043200"/>
+        <c:crossAx val="115286528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -480,6 +474,451 @@
           <c:y val="0.20514281536391318"/>
           <c:w val="9.5871673065660176E-2"/>
           <c:h val="0.19441451773416904"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" altLang="en-US" sz="2000"/>
+              <a:t>Performance Comparison (scaled)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1889215427997151"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2078523548868659"/>
+          <c:y val="0.25313684747739867"/>
+          <c:w val="0.74211047039194444"/>
+          <c:h val="0.53090873031454788"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2369.6799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2192.9899999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2457.0100000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1821.51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1109.8800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1234.58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1051.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>698.32500000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>223.96299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70.2149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3571.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>709.72400000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.53899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.2517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0843800000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6013099999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="103612992"/>
+        <c:axId val="103612416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="103612992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" altLang="ja-JP" sz="1800" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Planets</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1600">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103612416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="103612416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" altLang="ja-JP" sz="1800" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Frames Per Second</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1600">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.9801637248875489E-2"/>
+              <c:y val="0.25313684747739867"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103612992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79747192381621457"/>
+          <c:y val="0.25556401483621766"/>
+          <c:w val="0.12889413823272092"/>
+          <c:h val="0.18585707114672223"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -538,6 +977,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -835,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -947,9 +1416,6 @@
       <c r="B10">
         <v>698.32500000000005</v>
       </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
@@ -959,7 +1425,7 @@
         <v>223.96299999999999</v>
       </c>
       <c r="G11">
-        <v>5.44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -968,6 +1434,9 @@
       </c>
       <c r="B12">
         <v>70.2149</v>
+      </c>
+      <c r="G12">
+        <v>5.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>